<commit_message>
Updated sample data file in .xlsx and .ttl formats
</commit_message>
<xml_diff>
--- a/Rule_Learner/test_KG/(2024-07-29) - SemIIM - SampleDataFile (Test).xlsx
+++ b/Rule_Learner/test_KG/(2024-07-29) - SemIIM - SampleDataFile (Test).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mindika\FutureSoils\SemIIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53910599-D05F-4360-8B93-BC8A4AE12A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8D56B7-8509-4B06-8B15-66C15116F4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-60" windowWidth="29040" windowHeight="15720" tabRatio="486" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" tabRatio="486" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOIL" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="82">
   <si>
     <t>Site ID</t>
   </si>
@@ -246,9 +246,6 @@
   </si>
   <si>
     <t>Surface Applied</t>
-  </si>
-  <si>
-    <t>Incorporated by Sowing</t>
   </si>
   <si>
     <t>2020-05-22</t>
@@ -798,7 +795,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -853,15 +850,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1218,42 +1206,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29920CD-2C45-44ED-8B76-52970F42BD32}">
-  <dimension ref="A1:AG20"/>
+  <dimension ref="A1:AG19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="10.28515625" style="8" customWidth="1"/>
-    <col min="8" max="9" width="13.85546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="8"/>
+    <col min="7" max="7" width="10.26953125" style="8" customWidth="1"/>
+    <col min="8" max="9" width="13.81640625" style="8" customWidth="1"/>
     <col min="10" max="10" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.81640625" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.7265625" style="8" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="31" width="24.42578125" style="8" customWidth="1"/>
-    <col min="32" max="32" width="17.140625" style="8" customWidth="1"/>
+    <col min="23" max="31" width="24.453125" style="8" customWidth="1"/>
+    <col min="32" max="32" width="17.1796875" style="8" customWidth="1"/>
     <col min="33" max="33" width="18" style="8" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="8"/>
+    <col min="34" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1354,7 +1342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="5" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="5" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1380,10 +1368,10 @@
         <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>15</v>
@@ -1455,7 +1443,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="L3" s="6" t="s">
         <v>38</v>
       </c>
@@ -1508,18 +1496,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="F4" s="8">
         <v>1</v>
@@ -1528,13 +1516,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I4" s="8">
         <v>2666</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K4" s="14">
         <v>43983</v>
@@ -1584,18 +1572,18 @@
         <v>4.6096000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="F5" s="8">
         <v>1</v>
@@ -1604,13 +1592,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I5" s="8">
         <v>2666</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K5" s="14">
         <v>43983</v>
@@ -1660,18 +1648,18 @@
         <v>3.1476000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="F6" s="8">
         <v>2</v>
@@ -1680,13 +1668,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I6" s="8">
         <v>2666</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K6" s="14">
         <v>43983</v>
@@ -1736,18 +1724,18 @@
         <v>4.8676000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="F7" s="8">
         <v>2</v>
@@ -1756,13 +1744,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="8">
         <v>2666</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K7" s="14">
         <v>43983</v>
@@ -1812,36 +1800,35 @@
         <v>3.5947999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="19" t="s">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19">
-        <v>1</v>
-      </c>
-      <c r="G8" s="19">
-        <v>1</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="19">
+      <c r="I8" s="8">
         <v>2666</v>
       </c>
-      <c r="J8" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="21">
+      <c r="J8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="14">
         <v>44752</v>
       </c>
       <c r="L8" s="8">
@@ -1885,36 +1872,35 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="19" t="s">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19">
-        <v>1</v>
-      </c>
-      <c r="G9" s="19">
-        <v>1</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="19">
+      <c r="I9" s="8">
         <v>2666</v>
       </c>
-      <c r="J9" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K9" s="21">
+      <c r="J9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="14">
         <v>44752</v>
       </c>
       <c r="L9" s="8">
@@ -1958,36 +1944,35 @@
         <v>2.7004000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="19" t="s">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="F10" s="8">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19">
-        <v>2</v>
-      </c>
-      <c r="G10" s="19">
-        <v>1</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="19">
+      <c r="I10" s="8">
         <v>2666</v>
       </c>
-      <c r="J10" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="21">
+      <c r="J10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K10" s="14">
         <v>44752</v>
       </c>
       <c r="L10" s="8">
@@ -2031,36 +2016,35 @@
         <v>4.2312000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="19" t="s">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19">
-        <v>2</v>
-      </c>
-      <c r="G11" s="19">
-        <v>1</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="19">
+      <c r="I11" s="8">
         <v>2666</v>
       </c>
-      <c r="J11" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="21">
+      <c r="J11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" s="14">
         <v>44752</v>
       </c>
       <c r="L11" s="8">
@@ -2104,36 +2088,35 @@
         <v>3.3024</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="19" t="s">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19">
+      <c r="F12" s="8">
         <v>1</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="8">
         <v>2</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="19">
+      <c r="H12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="8">
         <v>2666</v>
       </c>
-      <c r="J12" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12" s="21">
+      <c r="J12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="14">
         <v>44752</v>
       </c>
       <c r="L12" s="8">
@@ -2177,36 +2160,35 @@
         <v>3.4228000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="19" t="s">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19">
+      <c r="F13" s="8">
         <v>1</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="8">
         <v>2</v>
       </c>
-      <c r="H13" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="19">
+      <c r="H13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="8">
         <v>2666</v>
       </c>
-      <c r="J13" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="J13" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="14">
         <v>44752</v>
       </c>
       <c r="L13" s="8">
@@ -2250,36 +2232,35 @@
         <v>2.4767999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="19" t="s">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19">
+      <c r="F14" s="8">
         <v>2</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="8">
         <v>2</v>
       </c>
-      <c r="H14" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="19">
+      <c r="H14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="8">
         <v>2666</v>
       </c>
-      <c r="J14" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K14" s="21">
+      <c r="J14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="14">
         <v>44752</v>
       </c>
       <c r="L14" s="8">
@@ -2323,36 +2304,35 @@
         <v>5.2632000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="19" t="s">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19">
+      <c r="F15" s="8">
         <v>2</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="8">
         <v>2</v>
       </c>
-      <c r="H15" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="19">
+      <c r="H15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="8">
         <v>2666</v>
       </c>
-      <c r="J15" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" s="21">
+      <c r="J15" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="14">
         <v>44752</v>
       </c>
       <c r="L15" s="8">
@@ -2396,36 +2376,35 @@
         <v>3.1992000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="19" t="s">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19">
+      <c r="F16" s="8">
         <v>1</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="8">
         <v>3</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="I16" s="19">
+      <c r="H16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="8">
         <v>2666</v>
       </c>
-      <c r="J16" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K16" s="21">
+      <c r="J16" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="14">
         <v>44752</v>
       </c>
       <c r="L16" s="8">
@@ -2469,36 +2448,35 @@
         <v>3.5603999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="19" t="s">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19">
+      <c r="F17" s="8">
         <v>1</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="8">
         <v>3</v>
       </c>
-      <c r="H17" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="I17" s="19">
+      <c r="H17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="8">
         <v>2666</v>
       </c>
-      <c r="J17" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K17" s="21">
+      <c r="J17" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="14">
         <v>44752</v>
       </c>
       <c r="L17" s="8">
@@ -2542,36 +2520,35 @@
         <v>2.7347999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="19" t="s">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19">
+      <c r="F18" s="8">
         <v>2</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="8">
         <v>3</v>
       </c>
-      <c r="H18" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="I18" s="19">
+      <c r="H18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="8">
         <v>2666</v>
       </c>
-      <c r="J18" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18" s="21">
+      <c r="J18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18" s="14">
         <v>44752</v>
       </c>
       <c r="L18" s="8">
@@ -2615,36 +2592,35 @@
         <v>4.9708000000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="19" t="s">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19">
+      <c r="F19" s="8">
         <v>2</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="8">
         <v>3</v>
       </c>
-      <c r="H19" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="I19" s="19">
+      <c r="H19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="8">
         <v>2666</v>
       </c>
-      <c r="J19" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K19" s="21">
+      <c r="J19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K19" s="14">
         <v>44752</v>
       </c>
       <c r="L19" s="8">
@@ -2687,19 +2663,6 @@
       <c r="AG19" s="15">
         <v>3.4744000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:AF7">
@@ -2716,40 +2679,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11B656F-68F6-4B50-8FDD-AB7F9C088F64}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="2"/>
-    <col min="13" max="13" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="2"/>
+    <col min="13" max="13" width="10.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="20.42578125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="2"/>
+    <col min="15" max="15" width="13.81640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="21.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="20.453125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="20.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2841,7 +2804,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2933,7 +2896,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -2970,37 +2933,37 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="19" t="s">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19">
-        <v>1</v>
-      </c>
-      <c r="G4" s="19">
-        <v>1</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" s="19">
+      <c r="I4" s="8">
         <v>2666</v>
       </c>
-      <c r="J4" s="19" t="s">
-        <v>79</v>
+      <c r="J4" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>67</v>
@@ -3011,41 +2974,38 @@
       <c r="P4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="W4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="8">
+        <v>2666</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="17" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19">
-        <v>2</v>
-      </c>
-      <c r="G5" s="19">
-        <v>1</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="19">
-        <v>2666</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>67</v>
@@ -3056,41 +3016,38 @@
       <c r="P5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="W5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2666</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19">
-        <v>1</v>
-      </c>
-      <c r="G6" s="19">
-        <v>2</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="19">
-        <v>2666</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>67</v>
@@ -3107,41 +3064,38 @@
       <c r="V6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8">
+        <v>2</v>
+      </c>
+      <c r="G7" s="8">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2666</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19">
-        <v>2</v>
-      </c>
-      <c r="G7" s="19">
-        <v>2</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="19">
-        <v>2666</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>67</v>
@@ -3158,41 +3112,38 @@
       <c r="V7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="8">
+        <v>2666</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19">
-        <v>1</v>
-      </c>
-      <c r="G8" s="19">
-        <v>3</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="19">
-        <v>2666</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>67</v>
@@ -3210,43 +3161,43 @@
         <v>70</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X8" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="19" t="s">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
         <v>2</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="8">
         <v>3</v>
       </c>
-      <c r="H9" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="I9" s="19">
+      <c r="H9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="8">
         <v>2666</v>
       </c>
-      <c r="J9" s="19" t="s">
-        <v>79</v>
+      <c r="J9" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>67</v>
@@ -3264,7 +3215,7 @@
         <v>70</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X9" s="2">
         <v>10</v>

</xml_diff>